<commit_message>
Added GUI functionality for template pages
Updates:
- Added Template Menu 
- Added Excel data binding to Template Menu
- Created Template BOIP detail intake page
- Created Template BOIP date intake page
- Linked Template Pages to Update Page
</commit_message>
<xml_diff>
--- a/boip creation tool/Utils/templatedata.xlsx
+++ b/boip creation tool/Utils/templatedata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tre\Documents\repo\boip creation tool\Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD6DC29-1D7B-4060-9800-5186FDAF532E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37306FFD-BEC7-4759-B080-83E16746449B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="270" windowWidth="21600" windowHeight="11385" xr2:uid="{017E4893-D0C5-4021-8558-1F7B0CBBC5FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{017E4893-D0C5-4021-8558-1F7B0CBBC5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Template Type</t>
   </si>
@@ -66,7 +66,22 @@
     <t>Dictionary</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>Custom_Release</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>Full_Install</t>
+  </si>
+  <si>
+    <t>Dictionary_Only</t>
+  </si>
+  <si>
+    <t>Dictionary_Metadata_EditClar</t>
+  </si>
+  <si>
+    <t>Dictionary_Clinical_Notes</t>
   </si>
 </sst>
 </file>
@@ -97,24 +112,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -154,15 +157,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -483,13 +482,14 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
@@ -500,18 +500,18 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -521,19 +521,19 @@
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>3</v>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,40 +543,45 @@
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>4</v>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>5</v>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>